<commit_message>
Finalized objects OLR for a test ingest
</commit_message>
<xml_diff>
--- a/amazonia/OLR/xls_standard_input_amazonia-objects.xlsx
+++ b/amazonia/OLR/xls_standard_input_amazonia-objects.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="734">
   <si>
     <t>text</t>
   </si>
@@ -2026,12 +2026,6 @@
   </si>
   <si>
     <t>0001</t>
-  </si>
-  <si>
-    <t>1616 - 1776 Colonial Era Forts  Military Presence.kmz</t>
-  </si>
-  <si>
-    <t>Colonial Era Forts</t>
   </si>
   <si>
     <t>Fort Island/ Kyk Overal (Dutch Fort)</t>
@@ -2067,6 +2061,9 @@
   </si>
   <si>
     <t>Colonial Era Forts.tiff</t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
   <si>
     <t>Real Forte Príncipe da Beira.tiff</t>
@@ -2363,7 +2360,16 @@
     <t>Summary Mapping File</t>
   </si>
   <si>
-    <t>Fort São Jose do Rio Negro, Amazonas Brazil.kmz</t>
+    <t>Colonial Era Forts.kmz</t>
+  </si>
+  <si>
+    <t>Santo Antônio do Gurupá (Founded as Mariocai by the Dutch).kmz</t>
+  </si>
+  <si>
+    <t>Sub-component</t>
+  </si>
+  <si>
+    <t>KMZ</t>
   </si>
 </sst>
 </file>
@@ -2989,7 +2995,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3033,15 +3039,6 @@
     <xf numFmtId="49" fontId="28" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="16" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3442,11 +3439,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J11" sqref="J11"/>
+      <selection pane="topRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,14 +3460,13 @@
     <col min="11" max="11" width="14.7109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
-    <col min="14" max="15" width="39.140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="42.85546875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="38.140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="20.5703125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="110.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="39.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="42.85546875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="38.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="110.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>338</v>
       </c>
@@ -3514,22 +3510,16 @@
         <v>4</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>347</v>
+        <v>455</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="Q1" s="23" t="s">
-        <v>460</v>
-      </c>
-      <c r="R1" s="23" t="s">
-        <v>623</v>
-      </c>
-      <c r="S1" s="23" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>630</v>
       </c>
@@ -3540,46 +3530,40 @@
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="H2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20" t="s">
+        <v>665</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>660</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>678</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>679</v>
+      </c>
+      <c r="N2"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20" t="s">
         <v>666</v>
       </c>
-      <c r="K2" s="20" t="s">
-        <v>661</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>679</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>680</v>
-      </c>
-      <c r="N2" t="s">
-        <v>645</v>
-      </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20" t="s">
-        <v>667</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S2" s="20"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q2" s="20"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D3" t="s">
         <v>359</v>
@@ -3589,7 +3573,7 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -3597,22 +3581,22 @@
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
-      <c r="N3"/>
+      <c r="N3" t="s">
+        <v>644</v>
+      </c>
       <c r="O3"/>
       <c r="P3"/>
       <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>631</v>
+        <v>730</v>
       </c>
       <c r="D4" t="s">
         <v>403</v>
@@ -3622,7 +3606,7 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -3630,68 +3614,62 @@
       <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>
-      <c r="N4"/>
+      <c r="N4" t="s">
+        <v>644</v>
+      </c>
       <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-    </row>
-    <row r="5" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B5" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="20" t="s">
+        <v>694</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20" t="s">
         <v>695</v>
       </c>
-      <c r="K5" s="20" t="s">
-        <v>661</v>
-      </c>
-      <c r="L5" s="20" t="s">
+      <c r="M5" s="20" t="s">
         <v>696</v>
       </c>
-      <c r="M5" s="20" t="s">
-        <v>697</v>
-      </c>
       <c r="N5" s="20" t="s">
-        <v>646</v>
-      </c>
-      <c r="O5" s="20"/>
+        <v>645</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>669</v>
+      </c>
       <c r="P5" s="20" t="s">
         <v>670</v>
       </c>
       <c r="Q5" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="R5" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S5" s="20" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B6" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D6" t="s">
         <v>359</v>
@@ -3700,7 +3678,9 @@
         <v>341</v>
       </c>
       <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
+      <c r="G6" s="20" t="s">
+        <v>642</v>
+      </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
@@ -3711,18 +3691,16 @@
       <c r="O6" s="20"/>
       <c r="P6" s="20"/>
       <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-    </row>
-    <row r="7" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B7" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D7" t="s">
         <v>403</v>
@@ -3731,7 +3709,9 @@
         <v>473</v>
       </c>
       <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="20" t="s">
+        <v>733</v>
+      </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
@@ -3742,65 +3722,57 @@
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-    </row>
-    <row r="8" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B8" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="20" t="s">
-        <v>652</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>661</v>
-      </c>
+        <v>651</v>
+      </c>
+      <c r="K8" s="20"/>
       <c r="L8" s="20" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>647</v>
-      </c>
-      <c r="O8" s="20"/>
+        <v>646</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>667</v>
+      </c>
       <c r="P8" s="20" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="R8" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S8" s="20" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B9" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D9" t="s">
         <v>359</v>
@@ -3809,7 +3781,9 @@
         <v>341</v>
       </c>
       <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="20" t="s">
+        <v>642</v>
+      </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
@@ -3820,18 +3794,16 @@
       <c r="O9" s="20"/>
       <c r="P9" s="20"/>
       <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-    </row>
-    <row r="10" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B10" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D10" t="s">
         <v>403</v>
@@ -3840,7 +3812,9 @@
         <v>473</v>
       </c>
       <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="20" t="s">
+        <v>733</v>
+      </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
@@ -3851,65 +3825,57 @@
       <c r="O10" s="20"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-    </row>
-    <row r="11" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B11" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="20" t="s">
-        <v>653</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>661</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="K11" s="20"/>
       <c r="L11" s="20" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>648</v>
-      </c>
-      <c r="O11" s="20"/>
+        <v>647</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>676</v>
+      </c>
       <c r="P11" s="20" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="Q11" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="R11" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S11" s="20" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B12" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D12" t="s">
         <v>359</v>
@@ -3918,7 +3884,9 @@
         <v>341</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="20" t="s">
+        <v>642</v>
+      </c>
       <c r="H12" s="21"/>
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
@@ -3929,18 +3897,16 @@
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-    </row>
-    <row r="13" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B13" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D13" t="s">
         <v>403</v>
@@ -3949,7 +3915,9 @@
         <v>473</v>
       </c>
       <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="20" t="s">
+        <v>733</v>
+      </c>
       <c r="H13" s="21"/>
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
@@ -3960,65 +3928,57 @@
       <c r="O13" s="20"/>
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-    </row>
-    <row r="14" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I14" s="20"/>
       <c r="J14" s="20" t="s">
-        <v>654</v>
-      </c>
-      <c r="K14" s="20" t="s">
-        <v>661</v>
-      </c>
+        <v>653</v>
+      </c>
+      <c r="K14" s="20"/>
       <c r="L14" s="20" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>649</v>
-      </c>
-      <c r="O14" s="20"/>
+        <v>648</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>668</v>
+      </c>
       <c r="P14" s="20" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="Q14" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="R14" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S14" s="20" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B15" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D15" t="s">
         <v>359</v>
@@ -4027,7 +3987,9 @@
         <v>341</v>
       </c>
       <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="20" t="s">
+        <v>642</v>
+      </c>
       <c r="H15" s="21"/>
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
@@ -4038,18 +4000,16 @@
       <c r="O15" s="20"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-    </row>
-    <row r="16" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B16" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D16" t="s">
         <v>403</v>
@@ -4058,7 +4018,9 @@
         <v>473</v>
       </c>
       <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="G16" s="20" t="s">
+        <v>733</v>
+      </c>
       <c r="H16" s="21"/>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
@@ -4069,65 +4031,57 @@
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-    </row>
-    <row r="17" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B17" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
       <c r="G17" s="20" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I17" s="20"/>
       <c r="J17" s="20" t="s">
-        <v>655</v>
-      </c>
-      <c r="K17" s="20" t="s">
-        <v>661</v>
-      </c>
+        <v>654</v>
+      </c>
+      <c r="K17" s="20"/>
       <c r="L17" s="20" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>650</v>
-      </c>
-      <c r="O17" s="20"/>
+        <v>649</v>
+      </c>
+      <c r="O17" s="20" t="s">
+        <v>675</v>
+      </c>
       <c r="P17" s="20" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="Q17" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="R17" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S17" s="20" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B18" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D18" t="s">
         <v>359</v>
@@ -4136,7 +4090,9 @@
         <v>341</v>
       </c>
       <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
+      <c r="G18" s="20" t="s">
+        <v>642</v>
+      </c>
       <c r="H18" s="21"/>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
@@ -4147,18 +4103,16 @@
       <c r="O18" s="20"/>
       <c r="P18" s="20"/>
       <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-    </row>
-    <row r="19" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B19" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D19" t="s">
         <v>403</v>
@@ -4167,7 +4121,9 @@
         <v>473</v>
       </c>
       <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+      <c r="G19" s="20" t="s">
+        <v>733</v>
+      </c>
       <c r="H19" s="21"/>
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
@@ -4178,67 +4134,59 @@
       <c r="O19" s="20"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-    </row>
-    <row r="20" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B20" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H20" s="21" t="s">
+        <v>661</v>
+      </c>
+      <c r="I20" s="20" t="s">
         <v>662</v>
       </c>
-      <c r="I20" s="20" t="s">
-        <v>663</v>
-      </c>
       <c r="J20" s="20" t="s">
-        <v>656</v>
-      </c>
-      <c r="K20" s="20" t="s">
-        <v>661</v>
-      </c>
+        <v>655</v>
+      </c>
+      <c r="K20" s="20"/>
       <c r="L20" s="20" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="O20" s="20"/>
+        <v>650</v>
+      </c>
+      <c r="O20" s="20" t="s">
+        <v>674</v>
+      </c>
       <c r="P20" s="20" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="Q20" s="20" t="s">
-        <v>672</v>
-      </c>
-      <c r="R20" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S20" s="20" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B21" t="s">
+        <v>732</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>715</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>716</v>
       </c>
       <c r="D21" t="s">
         <v>359</v>
@@ -4247,7 +4195,9 @@
         <v>341</v>
       </c>
       <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
+      <c r="G21" s="20" t="s">
+        <v>642</v>
+      </c>
       <c r="H21" s="21"/>
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
@@ -4258,18 +4208,16 @@
       <c r="O21" s="20"/>
       <c r="P21" s="20"/>
       <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-    </row>
-    <row r="22" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B22" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D22" t="s">
         <v>403</v>
@@ -4278,7 +4226,9 @@
         <v>473</v>
       </c>
       <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
+      <c r="G22" s="20" t="s">
+        <v>733</v>
+      </c>
       <c r="H22" s="21"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
@@ -4289,67 +4239,59 @@
       <c r="O22" s="20"/>
       <c r="P22" s="20"/>
       <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-    </row>
-    <row r="23" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B23" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I23" s="20" t="s">
+        <v>663</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>656</v>
+      </c>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20" t="s">
+        <v>701</v>
+      </c>
+      <c r="M23" s="20" t="s">
+        <v>692</v>
+      </c>
+      <c r="N23" s="20" t="s">
         <v>664</v>
       </c>
-      <c r="J23" s="20" t="s">
-        <v>657</v>
-      </c>
-      <c r="K23" s="20" t="s">
-        <v>661</v>
-      </c>
-      <c r="L23" s="20" t="s">
-        <v>702</v>
-      </c>
-      <c r="M23" s="20" t="s">
-        <v>693</v>
-      </c>
-      <c r="N23" s="20" t="s">
-        <v>665</v>
-      </c>
-      <c r="O23" s="20"/>
+      <c r="O23" s="20" t="s">
+        <v>674</v>
+      </c>
       <c r="P23" s="20" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="Q23" s="20" t="s">
-        <v>672</v>
-      </c>
-      <c r="R23" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S23" s="20" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B24" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D24" t="s">
         <v>359</v>
@@ -4358,7 +4300,9 @@
         <v>341</v>
       </c>
       <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
+      <c r="G24" s="20" t="s">
+        <v>642</v>
+      </c>
       <c r="H24" s="21"/>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
@@ -4369,18 +4313,16 @@
       <c r="O24" s="20"/>
       <c r="P24" s="20"/>
       <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="20"/>
-    </row>
-    <row r="25" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B25" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D25" t="s">
         <v>403</v>
@@ -4389,7 +4331,9 @@
         <v>473</v>
       </c>
       <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
+      <c r="G25" s="20" t="s">
+        <v>733</v>
+      </c>
       <c r="H25" s="21"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
@@ -4400,63 +4344,55 @@
       <c r="O25" s="20"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-    </row>
-    <row r="26" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B26" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="I26" s="20"/>
       <c r="J26" s="20" t="s">
-        <v>658</v>
-      </c>
-      <c r="K26" s="20" t="s">
-        <v>661</v>
-      </c>
+        <v>657</v>
+      </c>
+      <c r="K26" s="20"/>
       <c r="L26" s="20" t="s">
+        <v>702</v>
+      </c>
+      <c r="M26" s="20" t="s">
         <v>703</v>
       </c>
-      <c r="M26" s="20" t="s">
-        <v>704</v>
-      </c>
       <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
+      <c r="O26" s="20" t="s">
+        <v>673</v>
+      </c>
       <c r="P26" s="20" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="Q26" s="20" t="s">
-        <v>673</v>
-      </c>
-      <c r="R26" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S26" s="20" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B27" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D27" t="s">
         <v>359</v>
@@ -4465,7 +4401,9 @@
         <v>341</v>
       </c>
       <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
+      <c r="G27" s="20" t="s">
+        <v>642</v>
+      </c>
       <c r="H27" s="21"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
@@ -4476,18 +4414,16 @@
       <c r="O27" s="20"/>
       <c r="P27" s="20"/>
       <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-    </row>
-    <row r="28" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B28" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D28" t="s">
         <v>403</v>
@@ -4496,7 +4432,9 @@
         <v>473</v>
       </c>
       <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
+      <c r="G28" s="20" t="s">
+        <v>733</v>
+      </c>
       <c r="H28" s="21"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -4507,63 +4445,55 @@
       <c r="O28" s="20"/>
       <c r="P28" s="20"/>
       <c r="Q28" s="20"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-    </row>
-    <row r="29" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B29" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="I29" s="20"/>
       <c r="J29" s="20" t="s">
-        <v>659</v>
-      </c>
-      <c r="K29" s="20" t="s">
-        <v>661</v>
-      </c>
+        <v>658</v>
+      </c>
+      <c r="K29" s="20"/>
       <c r="L29" s="20" t="s">
+        <v>704</v>
+      </c>
+      <c r="M29" s="20" t="s">
         <v>705</v>
       </c>
-      <c r="M29" s="20" t="s">
-        <v>706</v>
-      </c>
       <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
+      <c r="O29" s="20" t="s">
+        <v>673</v>
+      </c>
       <c r="P29" s="20" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="Q29" s="20" t="s">
-        <v>673</v>
-      </c>
-      <c r="R29" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="S29" s="20" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B30" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D30" t="s">
         <v>359</v>
@@ -4572,7 +4502,9 @@
         <v>341</v>
       </c>
       <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
+      <c r="G30" s="20" t="s">
+        <v>642</v>
+      </c>
       <c r="H30" s="21"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -4583,18 +4515,16 @@
       <c r="O30" s="20"/>
       <c r="P30" s="20"/>
       <c r="Q30" s="20"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="20"/>
-    </row>
-    <row r="31" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B31" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D31" t="s">
         <v>403</v>
@@ -4603,7 +4533,9 @@
         <v>473</v>
       </c>
       <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
+      <c r="G31" s="20" t="s">
+        <v>733</v>
+      </c>
       <c r="H31" s="21"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -4614,63 +4546,55 @@
       <c r="O31" s="20"/>
       <c r="P31" s="20"/>
       <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-    </row>
-    <row r="32" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>630</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>715</v>
-      </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25" t="s">
-        <v>640</v>
-      </c>
-      <c r="H32" s="27" t="s">
-        <v>662</v>
-      </c>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25" t="s">
-        <v>660</v>
-      </c>
-      <c r="K32" s="25" t="s">
+      <c r="B32" t="s">
+        <v>714</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32" t="s">
+        <v>638</v>
+      </c>
+      <c r="H32" t="s">
         <v>661</v>
       </c>
-      <c r="L32" s="25" t="s">
-        <v>707</v>
-      </c>
-      <c r="M32" s="25" t="s">
-        <v>694</v>
-      </c>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="25" t="s">
-        <v>678</v>
-      </c>
-      <c r="Q32" s="25" t="s">
-        <v>671</v>
-      </c>
-      <c r="R32" s="25" t="s">
-        <v>632</v>
-      </c>
-      <c r="S32" s="25" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I32"/>
+      <c r="J32" t="s">
+        <v>659</v>
+      </c>
+      <c r="K32"/>
+      <c r="L32" t="s">
+        <v>706</v>
+      </c>
+      <c r="M32" t="s">
+        <v>693</v>
+      </c>
+      <c r="N32"/>
+      <c r="O32" t="s">
+        <v>677</v>
+      </c>
+      <c r="P32" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B33" t="s">
-        <v>715</v>
+        <v>732</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D33" t="s">
         <v>359</v>
@@ -4678,13 +4602,19 @@
       <c r="E33" s="3" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G33" s="20" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>630</v>
       </c>
       <c r="B34" t="s">
-        <v>715</v>
+        <v>732</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>731</v>
       </c>
       <c r="D34" t="s">
         <v>403</v>
@@ -4692,38 +4622,12 @@
       <c r="E34" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="29"/>
-      <c r="S35" s="29"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>715</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>731</v>
+      <c r="G34" s="20" t="s">
+        <v>733</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B35 B37:B1048576">
+  <conditionalFormatting sqref="B1 B35:B1048576">
     <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="    \Sub-component">
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
@@ -4740,7 +4644,7 @@
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list" sqref="B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="F1"/>
   </dataValidations>
@@ -4749,7 +4653,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
@@ -4772,13 +4676,13 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>P1:R1</xm:sqref>
+          <xm:sqref>O1:P1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>S1</xm:sqref>
+          <xm:sqref>Q1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -4790,13 +4694,13 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>N1:O1</xm:sqref>
+          <xm:sqref>N1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B35 B37:B1048576</xm:sqref>
+          <xm:sqref>B35:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>

</xml_diff>